<commit_message>
Add commit with 241119 History
</commit_message>
<xml_diff>
--- a/A comparative study of different features extracted from EIS in SoH for LIB/paper/Broadband_model_performance.xlsx
+++ b/A comparative study of different features extracted from EIS in SoH for LIB/paper/Broadband_model_performance.xlsx
@@ -5,22 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeongbs1\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeongbs1\오토실리콘\1. python_code\Practice_with_paper_data_sets\A comparative study of different features extracted from EIS in SoH for LIB\paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC2B635-9CE9-403E-B69B-93170581054E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E9CB8B-EF61-4424-8382-F79DFD62B81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Maximum Absolute Error (%)</t>
   </si>
@@ -50,6 +63,14 @@
   </si>
   <si>
     <t>Cell Name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Implementation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Paper</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -57,7 +78,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +100,15 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -88,7 +118,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -111,16 +141,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -425,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A2:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -442,107 +484,231 @@
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2">
-        <v>2.4463947392416721</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1.0384901974838729</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1.247626768106483</v>
-      </c>
-      <c r="E2" s="2">
-        <v>87.5</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1.306843803514161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2.1222690586859239</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.94943655175911323</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1.084367895570953</v>
-      </c>
-      <c r="E3" s="2">
-        <v>72.222222222222214</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.72052903748817732</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>2.091353785598812</v>
+        <v>2.5059999999999998</v>
       </c>
       <c r="C4" s="2">
-        <v>0.9867579185787545</v>
+        <v>0.88</v>
       </c>
       <c r="D4" s="2">
-        <v>1.125602132394953</v>
+        <v>1.101</v>
       </c>
       <c r="E4" s="2">
-        <v>73.68421052631578</v>
+        <v>95</v>
       </c>
       <c r="F4" s="2">
-        <v>0.84449781959157533</v>
+        <v>0.97499999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.9510000000000001</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.044</v>
+      </c>
+      <c r="E5" s="2">
+        <v>75</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.67200000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.655</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="E6" s="2">
+        <v>76.316000000000003</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.73899999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B7" s="2">
+        <v>2.8090000000000002</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.462</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.62</v>
+      </c>
+      <c r="E7" s="2">
+        <v>46.875</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.83599999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2.4463947392416721</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.0384901974838729</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1.247626768106483</v>
+      </c>
+      <c r="E12" s="2">
+        <v>87.5</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1.306843803514161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2.1222690586859239</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.94943655175911323</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1.084367895570953</v>
+      </c>
+      <c r="E13" s="2">
+        <v>72.222222222222214</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.72052903748817732</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2.091353785598812</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.9867579185787545</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1.125602132394953</v>
+      </c>
+      <c r="E14" s="2">
+        <v>73.68421052631578</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.84449781959157533</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2">
         <v>3.406560168211695</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C15" s="2">
         <v>1.8701149586631991</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D15" s="2">
         <v>2.0545302800891321</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E15" s="2">
         <v>56.25</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F15" s="2">
         <v>1.0804184036391311</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A2:F2"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>